<commit_message>
cap nhat file Anh12.xlsx
</commit_message>
<xml_diff>
--- a/Anh12.xlsx
+++ b/Anh12.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\LTUDQL1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\LTUDQL1\DA-LTUDQL1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="C72" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,6 +1223,9 @@
       <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1235,6 +1238,9 @@
       <c r="C4" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1246,6 +1252,9 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,6 +1268,9 @@
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1271,6 +1283,9 @@
       <c r="C7" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1298,6 +1313,9 @@
       <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1310,6 +1328,9 @@
       <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1337,6 +1358,9 @@
       <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1349,6 +1373,9 @@
       <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1376,6 +1403,9 @@
       <c r="C15" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1388,6 +1418,9 @@
       <c r="C16" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1400,6 +1433,9 @@
       <c r="C17" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1412,6 +1448,9 @@
       <c r="C18" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1439,6 +1478,9 @@
       <c r="C20" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1451,6 +1493,9 @@
       <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1463,6 +1508,9 @@
       <c r="C22" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1490,6 +1538,9 @@
       <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1502,6 +1553,9 @@
       <c r="C25" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1514,6 +1568,9 @@
       <c r="C26" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1526,6 +1583,9 @@
       <c r="C27" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1538,6 +1598,9 @@
       <c r="C28" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1565,6 +1628,9 @@
       <c r="C30" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1577,6 +1643,9 @@
       <c r="C31" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1589,6 +1658,9 @@
       <c r="C32" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -1616,6 +1688,9 @@
       <c r="C34" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -1628,6 +1703,9 @@
       <c r="C35" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -1655,6 +1733,9 @@
       <c r="C37" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -1682,6 +1763,9 @@
       <c r="C39" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -1694,6 +1778,9 @@
       <c r="C40" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -1706,6 +1793,9 @@
       <c r="C41" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1718,6 +1808,9 @@
       <c r="C42" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -1745,6 +1838,9 @@
       <c r="C44" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -1756,6 +1852,9 @@
       </c>
       <c r="C45" s="2" t="s">
         <v>84</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,6 +1868,9 @@
       <c r="C46" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -1781,6 +1883,9 @@
       <c r="C47" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -1808,6 +1913,9 @@
       <c r="C49" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -1835,6 +1943,9 @@
       <c r="C51" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -1847,6 +1958,9 @@
       <c r="C52" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -1859,6 +1973,9 @@
       <c r="C53" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -1886,6 +2003,9 @@
       <c r="C55" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -1898,6 +2018,9 @@
       <c r="C56" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -1910,6 +2033,9 @@
       <c r="C57" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -1937,6 +2063,9 @@
       <c r="C59" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -1949,6 +2078,9 @@
       <c r="C60" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -1961,6 +2093,9 @@
       <c r="C61" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -1973,6 +2108,9 @@
       <c r="C62" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -2000,6 +2138,9 @@
       <c r="C64" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
@@ -2012,6 +2153,9 @@
       <c r="C65" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
@@ -2024,6 +2168,9 @@
       <c r="C66" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
@@ -2051,6 +2198,9 @@
       <c r="C68" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
@@ -2063,6 +2213,9 @@
       <c r="C69" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -2075,6 +2228,9 @@
       <c r="C70" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
@@ -2087,6 +2243,9 @@
       <c r="C71" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -2114,6 +2273,9 @@
       <c r="C73" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -2126,6 +2288,9 @@
       <c r="C74" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
@@ -2138,6 +2303,9 @@
       <c r="C75" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -2150,6 +2318,9 @@
       <c r="C76" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -2192,6 +2363,9 @@
       <c r="C79" s="2" t="s">
         <v>111</v>
       </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -2204,8 +2378,11 @@
       <c r="C80" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>20</v>
       </c>
@@ -2215,6 +2392,9 @@
       </c>
       <c r="C81" s="2" t="s">
         <v>113</v>
+      </c>
+      <c r="D81" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>